<commit_message>
Changes after MSU-IIT work.
</commit_message>
<xml_diff>
--- a/AddressingIssues.xlsx
+++ b/AddressingIssues.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="20115" windowHeight="9270" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="20115" windowHeight="9270" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pages" sheetId="1" r:id="rId1"/>
     <sheet name="Entry" sheetId="2" r:id="rId2"/>
     <sheet name="Content Per Page" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t>Read</t>
   </si>
@@ -169,6 +169,63 @@
   </si>
   <si>
     <t>Content per Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        /*      unsigned char   ss ;    // seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        unsigned char   mn ;    // minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        unsigned char   hh ;    // hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        unsigned char   md ;    // day in month, from 1 to 31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        unsigned char   wd ;    // day in week, monday=0, tuesday=1, .... sunday=6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        unsigned char   mo ;    // month number, from 1 to 12 (and not from 0 to 11 as with unix C time !)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        unsigned int    yy ;    // year Y2K compliant, from 1892 to 2038*/</t>
+  </si>
+  <si>
+    <t>case 255: return "*";</t>
+  </si>
+  <si>
+    <t>case 254: return "-";</t>
+  </si>
+  <si>
+    <t>case 253: return "/";</t>
+  </si>
+  <si>
+    <t>case 252: return "On";</t>
+  </si>
+  <si>
+    <t>case 251: return "Off";</t>
+  </si>
+  <si>
+    <t>case 250: return "";</t>
+  </si>
+  <si>
+    <t>ASTERISK = 255,</t>
+  </si>
+  <si>
+    <t>DASH = 254,</t>
+  </si>
+  <si>
+    <t>SLASH = 253,</t>
+  </si>
+  <si>
+    <t>ON = 252,</t>
+  </si>
+  <si>
+    <t>OFF = 251,</t>
+  </si>
+  <si>
+    <t>EMPTY = 250</t>
   </si>
 </sst>
 </file>
@@ -192,12 +249,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -273,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -297,6 +360,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,7 +658,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1074,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1087,7 +1151,7 @@
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1098,235 +1162,292 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="9">
         <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="9">
         <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="9">
         <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="9">
         <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="9">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="9">
         <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="9">
         <v>6</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="9">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="9">
         <v>8</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="9">
         <v>9</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="9">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="9">
         <v>11</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="9">
         <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="9">
         <v>13</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="9">
         <v>14</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="9">
         <v>15</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="9">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="9">
         <v>17</v>
       </c>
       <c r="C19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="9">
         <v>18</v>
       </c>
       <c r="C20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="9">
         <v>19</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="9">
         <v>20</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1338,7 +1459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed some more software issues.
</commit_message>
<xml_diff>
--- a/AddressingIssues.xlsx
+++ b/AddressingIssues.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="20115" windowHeight="9270" activeTab="1"/>
@@ -11,12 +11,12 @@
     <sheet name="Entry" sheetId="2" r:id="rId2"/>
     <sheet name="Content Per Page" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="91">
   <si>
     <t>Read</t>
   </si>
@@ -226,6 +226,69 @@
   </si>
   <si>
     <t>EMPTY = 250</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>mnl</t>
+  </si>
+  <si>
+    <t>mnc</t>
+  </si>
+  <si>
+    <t>mnu</t>
+  </si>
+  <si>
+    <t>hhl</t>
+  </si>
+  <si>
+    <t>hhc</t>
+  </si>
+  <si>
+    <t>hhu</t>
+  </si>
+  <si>
+    <t>mdl</t>
+  </si>
+  <si>
+    <t>mdc</t>
+  </si>
+  <si>
+    <t>mdu</t>
+  </si>
+  <si>
+    <t>wdl</t>
+  </si>
+  <si>
+    <t>wdc</t>
+  </si>
+  <si>
+    <t>wdu</t>
+  </si>
+  <si>
+    <t>mol</t>
+  </si>
+  <si>
+    <t>moc</t>
+  </si>
+  <si>
+    <t>mou</t>
+  </si>
+  <si>
+    <t>yyl</t>
+  </si>
+  <si>
+    <t>yyc</t>
+  </si>
+  <si>
+    <t>yyu</t>
   </si>
 </sst>
 </file>
@@ -342,6 +405,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -360,7 +424,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,38 +738,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
       <c r="M2" t="s">
         <v>8</v>
       </c>
@@ -1138,10 +1201,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2:R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1149,9 +1212,12 @@
     <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1162,11 +1228,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="3">
         <v>0</v>
       </c>
       <c r="C2" t="s">
@@ -1175,12 +1241,30 @@
       <c r="D2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="N2" t="str">
+        <f t="shared" ref="N2:N22" si="0">CONCATENATE("ADDR_",UPPER(C2), " = ",B2,",")</f>
+        <v>ADDR_ENABLE = 0,</v>
+      </c>
+      <c r="O2" t="str">
+        <f>CONCATENATE("ADDR_",UPPER(C2))</f>
+        <v>ADDR_ENABLE</v>
+      </c>
+      <c r="P2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2" t="str">
+        <f>CONCATENATE("entryStruct-&gt;",P2," = entry[",Q2,"]; // ", C2)</f>
+        <v>entryStruct-&gt;en = entry[0]; // Enable</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
@@ -1189,12 +1273,30 @@
       <c r="D3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="N3" t="str">
+        <f t="shared" si="0"/>
+        <v>ADDR_DEVICEID = 1,</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O22" si="1">CONCATENATE("ADDR_",UPPER(C3))</f>
+        <v>ADDR_DEVICEID</v>
+      </c>
+      <c r="P3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3" t="str">
+        <f t="shared" ref="R3:R22" si="2">CONCATENATE("entryStruct-&gt;",P3," = entry[",Q3,"]; // ", C3)</f>
+        <v>entryStruct-&gt;id = entry[1]; // DeviceID</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="3">
         <v>2</v>
       </c>
       <c r="C4" t="s">
@@ -1203,12 +1305,30 @@
       <c r="D4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="N4" t="str">
+        <f t="shared" si="0"/>
+        <v>ADDR_DEVICESTATE = 2,</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_DEVICESTATE</v>
+      </c>
+      <c r="P4" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;ds = entry[2]; // DeviceState</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="3">
         <v>3</v>
       </c>
       <c r="C5" t="s">
@@ -1217,26 +1337,62 @@
       <c r="D5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="N5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>ADDR_MINUTESLOWER = 3,</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_MINUTESLOWER</v>
+      </c>
+      <c r="P5" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q5">
+        <v>3</v>
+      </c>
+      <c r="R5" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;mnl = entry[3]; // MinutesLower</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="3">
         <v>4</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="N6" t="str">
+        <f t="shared" si="0"/>
+        <v>ADDR_MINUTESCLASSIFIER = 4,</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_MINUTESCLASSIFIER</v>
+      </c>
+      <c r="P6" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q6">
+        <v>4</v>
+      </c>
+      <c r="R6" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;mnc = entry[4]; // MinutesClassifier</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="3">
         <v>5</v>
       </c>
       <c r="C7" t="s">
@@ -1245,12 +1401,30 @@
       <c r="D7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="N7" t="str">
+        <f t="shared" si="0"/>
+        <v>ADDR_MINUTESUPPER = 5,</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_MINUTESUPPER</v>
+      </c>
+      <c r="P7" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q7">
+        <v>5</v>
+      </c>
+      <c r="R7" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;mnu = entry[5]; // MinutesUpper</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="3">
         <v>6</v>
       </c>
       <c r="C8" t="s">
@@ -1259,23 +1433,59 @@
       <c r="D8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="N8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>ADDR_HOURLOWER = 6,</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_HOURLOWER</v>
+      </c>
+      <c r="P8" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q8">
+        <v>6</v>
+      </c>
+      <c r="R8" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;hhl = entry[6]; // HourLower</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="3">
         <v>7</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="N9" t="str">
+        <f t="shared" si="0"/>
+        <v>ADDR_HOURCLASSIFIER = 7,</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_HOURCLASSIFIER</v>
+      </c>
+      <c r="P9" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q9">
+        <v>7</v>
+      </c>
+      <c r="R9" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;hhc = entry[7]; // HourClassifier</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="3">
         <v>8</v>
       </c>
       <c r="C10" t="s">
@@ -1284,12 +1494,30 @@
       <c r="D10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="N10" t="str">
+        <f t="shared" si="0"/>
+        <v>ADDR_HOURUPPER = 8,</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_HOURUPPER</v>
+      </c>
+      <c r="P10" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q10">
+        <v>8</v>
+      </c>
+      <c r="R10" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;hhu = entry[8]; // HourUpper</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="3">
         <v>9</v>
       </c>
       <c r="C11" t="s">
@@ -1298,26 +1526,62 @@
       <c r="D11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="N11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>ADDR_MONTHDAYLOWER = 9,</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_MONTHDAYLOWER</v>
+      </c>
+      <c r="P11" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q11">
+        <v>9</v>
+      </c>
+      <c r="R11" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;mdl = entry[9]; // MonthDayLower</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="3">
         <v>10</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="N12" t="str">
+        <f t="shared" si="0"/>
+        <v>ADDR_MONTHDAYCLASSIFIER = 10,</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_MONTHDAYCLASSIFIER</v>
+      </c>
+      <c r="P12" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q12">
+        <v>10</v>
+      </c>
+      <c r="R12" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;mdc = entry[10]; // MonthDayClassifier</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="3">
         <v>11</v>
       </c>
       <c r="C13" t="s">
@@ -1326,12 +1590,30 @@
       <c r="D13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="N13" t="str">
+        <f t="shared" si="0"/>
+        <v>ADDR_MONTHDAYUPPER = 11,</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_MONTHDAYUPPER</v>
+      </c>
+      <c r="P13" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q13">
+        <v>11</v>
+      </c>
+      <c r="R13" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;mdu = entry[11]; // MonthDayUpper</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="3">
         <v>12</v>
       </c>
       <c r="C14" t="s">
@@ -1340,37 +1622,91 @@
       <c r="D14" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="N14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>ADDR_WEEKDAYLOWER = 12,</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_WEEKDAYLOWER</v>
+      </c>
+      <c r="P14" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q14">
+        <v>12</v>
+      </c>
+      <c r="R14" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;wdl = entry[12]; // WeekdayLower</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="3">
         <v>13</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D15" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="N15" t="str">
+        <f t="shared" si="0"/>
+        <v>ADDR_WEEKDAYCLASSIFIER = 13,</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_WEEKDAYCLASSIFIER</v>
+      </c>
+      <c r="P15" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q15">
+        <v>13</v>
+      </c>
+      <c r="R15" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;wdc = entry[13]; // WeekdayClassifier</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="3">
         <v>14</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="N16" t="str">
+        <f t="shared" si="0"/>
+        <v>ADDR_WEEKDAYUPPER = 14,</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_WEEKDAYUPPER</v>
+      </c>
+      <c r="P16" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q16">
+        <v>14</v>
+      </c>
+      <c r="R16" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;wdu = entry[14]; // WeekdayUpper</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="3">
         <v>15</v>
       </c>
       <c r="C17" t="s">
@@ -1379,26 +1715,62 @@
       <c r="D17" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="N17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>ADDR_MONTHLOWER = 15,</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_MONTHLOWER</v>
+      </c>
+      <c r="P17" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q17">
+        <v>15</v>
+      </c>
+      <c r="R17" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;mol = entry[15]; // MonthLower</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="3">
         <v>16</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D18" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="N18" t="str">
+        <f>CONCATENATE("ADDR_",UPPER(C18), " = ",B18,",")</f>
+        <v>ADDR_MONTHCLASSIFIER = 16,</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_MONTHCLASSIFIER</v>
+      </c>
+      <c r="P18" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q18">
+        <v>16</v>
+      </c>
+      <c r="R18" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;moc = entry[16]; // MonthClassifier</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="3">
         <v>17</v>
       </c>
       <c r="C19" t="s">
@@ -1407,12 +1779,30 @@
       <c r="D19" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="N19" t="str">
+        <f t="shared" ref="N19:N22" si="3">CONCATENATE("ADDR_",UPPER(C19), " = ",B19,",")</f>
+        <v>ADDR_MONTHUPPER = 17,</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_MONTHUPPER</v>
+      </c>
+      <c r="P19" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q19">
+        <v>17</v>
+      </c>
+      <c r="R19" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;mou = entry[17]; // MonthUpper</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="3">
         <v>18</v>
       </c>
       <c r="C20" t="s">
@@ -1421,26 +1811,62 @@
       <c r="D20" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="N20" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>ADDR_YEARLOWER = 18,</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_YEARLOWER</v>
+      </c>
+      <c r="P20" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q20">
+        <v>18</v>
+      </c>
+      <c r="R20" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;yyl = entry[18]; // YearLower</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="3">
         <v>19</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D21" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="N21" t="str">
+        <f t="shared" si="3"/>
+        <v>ADDR_YEARCLASSIFIER = 19,</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_YEARCLASSIFIER</v>
+      </c>
+      <c r="P21" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q21">
+        <v>19</v>
+      </c>
+      <c r="R21" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;yyc = entry[19]; // YearClassifier</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="3">
         <v>20</v>
       </c>
       <c r="C22" t="s">
@@ -1448,6 +1874,24 @@
       </c>
       <c r="D22" t="s">
         <v>69</v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="3"/>
+        <v>ADDR_YEARUPPER = 20,</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="1"/>
+        <v>ADDR_YEARUPPER</v>
+      </c>
+      <c r="P22" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q22">
+        <v>20</v>
+      </c>
+      <c r="R22" t="str">
+        <f t="shared" si="2"/>
+        <v>entryStruct-&gt;yyu = entry[20]; // YearUpper</v>
       </c>
     </row>
   </sheetData>
@@ -1470,12 +1914,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">

</xml_diff>